<commit_message>
2018 fall - first half
</commit_message>
<xml_diff>
--- a/dm1/lecture/06/cartExample.xlsx
+++ b/dm1/lecture/06/cartExample.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AFMS\r\rn\rw\dm1\lecture\06\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19545" windowHeight="5820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -151,11 +156,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +210,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -497,27 +510,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="9" max="9" width="29.28515625" customWidth="1"/>
     <col min="12" max="12" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -525,7 +538,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -566,7 +579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -617,7 +630,7 @@
         <v>0.43750000000000011</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -650,7 +663,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:22">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -701,7 +714,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -734,7 +747,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -785,7 +798,7 @@
         <v>0.12499999999999997</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -818,7 +831,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -875,7 +888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:22">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -909,7 +922,7 @@
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I11" t="s">
         <v>12</v>
       </c>
@@ -945,7 +958,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2" t="s">
@@ -963,7 +976,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
         <v>13</v>
       </c>
@@ -999,7 +1012,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2" t="s">
@@ -1017,7 +1030,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:22">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
         <v>14</v>
       </c>
@@ -1053,7 +1066,7 @@
         <v>0.43750000000000011</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
       <c r="L16" s="2" t="s">
@@ -1071,7 +1084,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>15</v>
       </c>
@@ -1107,7 +1120,7 @@
         <v>0.12499999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:22">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2" t="s">
@@ -1125,7 +1138,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I19" t="s">
         <v>16</v>
       </c>
@@ -1161,7 +1174,7 @@
         <v>0.5625</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2" t="s">
@@ -1179,7 +1192,7 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
     </row>
-    <row r="23" spans="1:22">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>38</v>
       </c>
@@ -1187,7 +1200,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:22">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1241,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1278,7 +1291,7 @@
         <v>0.11111111111111109</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>39</v>
       </c>
@@ -1311,7 +1324,7 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
     </row>
-    <row r="27" spans="1:22">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3</v>
       </c>
@@ -1368,7 +1381,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:22">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>4</v>
       </c>
@@ -1402,7 +1415,7 @@
       <c r="P28" s="7"/>
       <c r="Q28" s="7"/>
     </row>
-    <row r="29" spans="1:22">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1453,7 +1466,7 @@
         <v>0.44444444444444448</v>
       </c>
     </row>
-    <row r="30" spans="1:22" ht="13.5" customHeight="1">
+    <row r="30" spans="1:22" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>6</v>
       </c>
@@ -1487,7 +1500,7 @@
       <c r="P30" s="3"/>
       <c r="Q30" s="3"/>
     </row>
-    <row r="31" spans="1:22">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>39</v>
       </c>
@@ -1538,7 +1551,7 @@
         <v>0.22222222222222224</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>8</v>
       </c>
@@ -1571,7 +1584,7 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
     </row>
-    <row r="33" spans="1:22">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I33" t="s">
         <v>13</v>
       </c>
@@ -1607,7 +1620,7 @@
         <v>0.22222222222222224</v>
       </c>
     </row>
-    <row r="34" spans="1:22">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2" t="s">
@@ -1625,7 +1638,7 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
     </row>
-    <row r="35" spans="1:22">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I35" t="s">
         <v>14</v>
       </c>
@@ -1661,7 +1674,7 @@
         <v>0.44444444444444448</v>
       </c>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2" t="s">
@@ -1679,7 +1692,7 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I37" t="s">
         <v>15</v>
       </c>
@@ -1714,7 +1727,7 @@
         <v>1.1937557392102845E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J38" s="2"/>
       <c r="K38" s="2"/>
       <c r="L38" s="2" t="s">
@@ -1732,7 +1745,7 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
     </row>
-    <row r="39" spans="1:22">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="I39" t="s">
         <v>16</v>
       </c>
@@ -1767,7 +1780,7 @@
         <v>5.7851239669421496E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:22">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="J40" s="2"/>
       <c r="K40" s="2"/>
       <c r="L40" s="2" t="s">
@@ -1785,7 +1798,7 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
     </row>
-    <row r="44" spans="1:22">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -1793,7 +1806,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -1834,7 +1847,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:22">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>39</v>
       </c>
@@ -1884,7 +1897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:22">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>39</v>
       </c>
@@ -1917,7 +1930,7 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
     </row>
-    <row r="48" spans="1:22">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>3</v>
       </c>
@@ -1973,7 +1986,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>39</v>
       </c>
@@ -2006,7 +2019,7 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>39</v>
       </c>
@@ -2023,7 +2036,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>6</v>
       </c>
@@ -2040,7 +2053,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:17">
+    <row r="52" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>39</v>
       </c>
@@ -2057,7 +2070,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>39</v>
       </c>
@@ -2074,7 +2087,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:17">
+    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
     </row>
   </sheetData>

</xml_diff>